<commit_message>
feat: enhance SupportAssistant with UX improvements
- Add rotating loading messages (5 variants, 600ms intervals)
- Implement persistent checklist with localStorage
- Add ShieldAlert icon to medical disclaimer (ZOL warning)
- Improve micro-copy throughout wizard flow
- Add visual polish (gradient on PDF card, better descriptions)
- Implement auto-start via ?start=true query param
- Add location field validation (min 2 chars required)
- Fix API endpoint error handling and logging
- Update button states (disabled when invalid input)

UX improvements based on Gemini design patterns
</commit_message>
<xml_diff>
--- a/raw_dane/malopolskie/Wykaz środowiskowych domów samopomocy(5).xlsx
+++ b/raw_dane/malopolskie/Wykaz środowiskowych domów samopomocy(5).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcebula\Desktop\Wykaz ŚDS\2026\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iwona/Documents/Projekty/kompas-seniora/raw_dane/malopolskie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDDFB6B7-B5A1-41B3-AA71-FC1E37CF438D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14DE8CB-78AD-2845-A024-338FD405684E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3419,7 +3428,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3507,7 +3516,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3534,7 +3543,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3579,7 +3588,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3592,7 +3601,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3606,7 +3615,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3886,25 +3895,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="162" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="73.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="73.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="30.5" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="10" width="27.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="10" width="27.83203125" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="74" t="s">
         <v>456</v>
       </c>
@@ -3919,7 +3928,7 @@
       <c r="J1" s="75"/>
       <c r="K1" s="76"/>
     </row>
-    <row r="2" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>0</v>
       </c>
@@ -3934,7 +3943,7 @@
       <c r="J2" s="78"/>
       <c r="K2" s="79"/>
     </row>
-    <row r="3" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3969,7 +3978,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -4000,7 +4009,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -4035,7 +4044,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4070,7 +4079,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -4105,7 +4114,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>5</v>
       </c>
@@ -4140,7 +4149,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>6</v>
       </c>
@@ -4175,7 +4184,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>7</v>
       </c>
@@ -4210,7 +4219,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>8</v>
       </c>
@@ -4245,7 +4254,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>9</v>
       </c>
@@ -4276,7 +4285,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
         <v>10</v>
       </c>
@@ -4309,7 +4318,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>11</v>
       </c>
@@ -4344,7 +4353,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
         <v>12</v>
       </c>
@@ -4375,7 +4384,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="98" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>13</v>
       </c>
@@ -4406,7 +4415,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
         <v>14</v>
       </c>
@@ -4441,7 +4450,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>15</v>
       </c>
@@ -4472,7 +4481,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
         <v>16</v>
       </c>
@@ -4507,7 +4516,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>17</v>
       </c>
@@ -4538,7 +4547,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
         <v>18</v>
       </c>
@@ -4569,7 +4578,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="98" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>19</v>
       </c>
@@ -4600,7 +4609,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="98" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <v>20</v>
       </c>
@@ -4631,7 +4640,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>21</v>
       </c>
@@ -4662,7 +4671,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A25" s="12">
         <v>22</v>
       </c>
@@ -4693,7 +4702,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>23</v>
       </c>
@@ -4724,7 +4733,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12">
         <v>24</v>
       </c>
@@ -4755,7 +4764,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>25</v>
       </c>
@@ -4786,7 +4795,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12">
         <v>26</v>
       </c>
@@ -4821,7 +4830,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>27</v>
       </c>
@@ -4852,7 +4861,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12">
         <v>28</v>
       </c>
@@ -4887,7 +4896,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>29</v>
       </c>
@@ -4922,7 +4931,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12">
         <v>30</v>
       </c>
@@ -4957,7 +4966,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="70" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>31</v>
       </c>
@@ -4988,7 +4997,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="12">
         <v>32</v>
       </c>
@@ -5023,7 +5032,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>33</v>
       </c>
@@ -5058,7 +5067,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="12">
         <v>34</v>
       </c>
@@ -5093,7 +5102,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="98" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>35</v>
       </c>
@@ -5124,7 +5133,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="12">
         <v>36</v>
       </c>
@@ -5159,7 +5168,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="98" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>37</v>
       </c>
@@ -5190,7 +5199,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="12">
         <v>38</v>
       </c>
@@ -5225,7 +5234,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>39</v>
       </c>
@@ -5260,7 +5269,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="12">
         <v>40</v>
       </c>
@@ -5293,7 +5302,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>41</v>
       </c>
@@ -5328,7 +5337,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="12">
         <v>42</v>
       </c>
@@ -5363,7 +5372,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>43</v>
       </c>
@@ -5398,7 +5407,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="12">
         <v>44</v>
       </c>
@@ -5433,7 +5442,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>45</v>
       </c>
@@ -5468,7 +5477,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="98" x14ac:dyDescent="0.2">
       <c r="A49" s="12">
         <v>46</v>
       </c>
@@ -5499,7 +5508,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="98" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>47</v>
       </c>
@@ -5530,7 +5539,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="98" x14ac:dyDescent="0.2">
       <c r="A51" s="12">
         <v>48</v>
       </c>
@@ -5563,7 +5572,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="98" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>49</v>
       </c>
@@ -5594,7 +5603,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="12">
         <v>50</v>
       </c>
@@ -5629,7 +5638,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>51</v>
       </c>
@@ -5660,7 +5669,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A55" s="12">
         <v>52</v>
       </c>
@@ -5691,7 +5700,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>53</v>
       </c>
@@ -5726,7 +5735,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="12">
         <v>54</v>
       </c>
@@ -5761,7 +5770,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>55</v>
       </c>
@@ -5792,7 +5801,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="12">
         <v>56</v>
       </c>
@@ -5827,7 +5836,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>57</v>
       </c>
@@ -5862,7 +5871,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="26"/>
       <c r="B61" s="27" t="s">
         <v>221</v>
@@ -5892,7 +5901,7 @@
       <c r="J61" s="64"/>
       <c r="K61" s="30"/>
     </row>
-    <row r="62" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="80" t="s">
         <v>223</v>
       </c>
@@ -5907,7 +5916,7 @@
       <c r="J62" s="81"/>
       <c r="K62" s="82"/>
     </row>
-    <row r="63" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>1</v>
       </c>
@@ -5940,7 +5949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="31">
         <v>58</v>
       </c>
@@ -5975,7 +5984,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="31">
         <v>59</v>
       </c>
@@ -6006,7 +6015,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="31">
         <v>60</v>
       </c>
@@ -6041,7 +6050,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A67" s="31">
         <v>61</v>
       </c>
@@ -6072,7 +6081,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A68" s="31">
         <v>62</v>
       </c>
@@ -6103,7 +6112,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A69" s="31">
         <v>63</v>
       </c>
@@ -6134,7 +6143,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="31">
         <v>64</v>
       </c>
@@ -6165,7 +6174,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A71" s="31">
         <v>65</v>
       </c>
@@ -6196,7 +6205,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A72" s="31">
         <v>66</v>
       </c>
@@ -6227,7 +6236,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A73" s="31">
         <v>67</v>
       </c>
@@ -6258,7 +6267,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="31">
         <v>68</v>
       </c>
@@ -6293,7 +6302,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="31">
         <v>69</v>
       </c>
@@ -6328,7 +6337,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="31">
         <v>70</v>
       </c>
@@ -6359,7 +6368,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A77" s="31">
         <v>71</v>
       </c>
@@ -6394,7 +6403,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="31">
         <v>72</v>
       </c>
@@ -6425,7 +6434,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="31">
         <v>73</v>
       </c>
@@ -6456,7 +6465,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="31">
         <v>74</v>
       </c>
@@ -6491,7 +6500,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="31">
         <v>75</v>
       </c>
@@ -6522,7 +6531,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="31">
         <v>76</v>
       </c>
@@ -6557,7 +6566,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="31">
         <v>77</v>
       </c>
@@ -6588,7 +6597,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="31">
         <v>78</v>
       </c>
@@ -6623,7 +6632,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="31">
         <v>79</v>
       </c>
@@ -6658,7 +6667,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="31">
         <v>80</v>
       </c>
@@ -6689,7 +6698,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="102" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="112" x14ac:dyDescent="0.2">
       <c r="A87" s="31">
         <v>81</v>
       </c>
@@ -6724,7 +6733,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="31">
         <v>82</v>
       </c>
@@ -6755,7 +6764,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="70" x14ac:dyDescent="0.2">
       <c r="A89" s="31">
         <v>83</v>
       </c>
@@ -6786,7 +6795,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="31">
         <v>84</v>
       </c>
@@ -6821,7 +6830,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A91" s="31">
         <v>85</v>
       </c>
@@ -6854,7 +6863,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="31">
         <v>86</v>
       </c>
@@ -6885,7 +6894,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="42"/>
       <c r="B93" s="43"/>
       <c r="C93" s="29"/>
@@ -6911,7 +6920,7 @@
       <c r="J93" s="29"/>
       <c r="K93" s="29"/>
     </row>
-    <row r="94" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="42"/>
       <c r="B94" s="43"/>
       <c r="C94" s="29"/>
@@ -6932,7 +6941,7 @@
       <c r="J94" s="29"/>
       <c r="K94" s="29"/>
     </row>
-    <row r="95" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="83" t="s">
         <v>330</v>
       </c>
@@ -6947,7 +6956,7 @@
       <c r="J95" s="84"/>
       <c r="K95" s="85"/>
     </row>
-    <row r="96" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A96" s="33" t="s">
         <v>10</v>
       </c>
@@ -6972,7 +6981,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="33" t="s">
         <v>16</v>
       </c>
@@ -6997,7 +7006,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="49"/>
       <c r="B98" s="50"/>
       <c r="C98" s="51"/>
@@ -7014,7 +7023,7 @@
       <c r="J98" s="66"/>
       <c r="K98" s="54"/>
     </row>
-    <row r="99" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="55"/>
       <c r="B99" s="86" t="s">
         <v>338</v>
@@ -7029,7 +7038,7 @@
       <c r="J99" s="87"/>
       <c r="K99" s="87"/>
     </row>
-    <row r="100" spans="1:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="56" t="s">
         <v>10</v>
       </c>
@@ -7054,7 +7063,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="71"/>
       <c r="B101" s="53"/>
       <c r="C101" s="72"/>
@@ -7071,7 +7080,7 @@
       <c r="J101" s="73"/>
       <c r="K101" s="72"/>
     </row>
-    <row r="102" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="70"/>
       <c r="B102" s="69"/>
       <c r="C102" s="68"/>

</xml_diff>